<commit_message>
Add doubletake different version
</commit_message>
<xml_diff>
--- a/doubletake/figure/performance.xlsx
+++ b/doubletake/figure/performance.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="12960" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20760" windowHeight="13700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Performance-SPEC2006" sheetId="4" r:id="rId1"/>
     <sheet name="Investigation" sheetId="7" r:id="rId2"/>
-    <sheet name="MemoryOverhead" sheetId="5" r:id="rId3"/>
-    <sheet name="Performance-Multithreading" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="Characteristics" sheetId="8" r:id="rId3"/>
+    <sheet name="MemoryOverhead" sheetId="5" r:id="rId4"/>
+    <sheet name="Performance-Multithreading" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
+  <si>
+    <t>Syscalls</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mallocs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOUBLETAKE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>433.milc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>470.lbm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OD+LD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Phoenix</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -176,11 +200,71 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>AVERAGE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>483.xalancbmk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressSanitizer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>287*3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>14hour</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valgrind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valgrind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valgrind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>447.dealII</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeakageDetection</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OverflowDetection</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>464.h264ref</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Original</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>AVERAGE</t>
+    <t>Use-After-FreeDetection</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllDetection</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -188,31 +272,47 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>400.perlbench</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>401.bzip2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>429.mcf</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>445.gobmk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>456.hmmer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>458.sjeng</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>471.omnetpp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>473.astar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>483.xalancbmk</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>AddressSanitizer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>287*3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>14hour</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valgrind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valgrind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valgrind</t>
+    <t>433.milc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>444.namd</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -220,119 +320,39 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>LeakageDetection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OverflowDetection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>All</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>DOUBLETAKE</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>OD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>482.sphinx3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>400.perlbench</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>403.gcc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>464.h264ref</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>AVERAGE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Original</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AddressSanitizer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Use-After-FreeDetection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AllDetection</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DoubleTake</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>400.perlbench</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>400.perlbench</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>401.bzip2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>403.gcc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>429.mcf</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>445.gobmk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>482.sphinx3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>456.hmmer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>458.sjeng</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>471.omnetpp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>473.astar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>483.xalancbmk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>433.milc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>444.namd</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>447.dealII</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overflow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overflow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overflow+MemoryLeak</t>
+    <t>Epochs</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -436,7 +456,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Original</c:v>
+                  <c:v>OD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -444,7 +464,7 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -523,64 +543,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1.351666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.962091503267974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.970540098199673</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.947136563876652</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.997329773030708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.994535519125683</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>0.997506234413965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>0.996920708237105</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1.036968576709797</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>0.97008547008547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0</c:v>
+                  <c:v>1.007989347536618</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0</c:v>
+                  <c:v>1.052023121387283</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0</c:v>
+                  <c:v>1.033707865168539</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0</c:v>
+                  <c:v>0.992199687987519</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0</c:v>
+                  <c:v>1.11660777385159</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0</c:v>
+                  <c:v>1.001492537313433</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0</c:v>
+                  <c:v>0.994169096209913</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0</c:v>
+                  <c:v>0.989556135770235</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0</c:v>
+                  <c:v>0.997534921939195</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0</c:v>
+                  <c:v>1.021582189514633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,7 +615,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AddressSanitizer</c:v>
+                  <c:v>OD+LD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -603,8 +623,8 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -683,64 +703,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.303333333333333</c:v>
+                  <c:v>1.306666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.231372549019608</c:v>
+                  <c:v>0.963398692810458</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.761047463175123</c:v>
+                  <c:v>0.970540098199673</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.048458149779736</c:v>
+                  <c:v>0.945668135095448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.21762349799733</c:v>
+                  <c:v>0.997329773030708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.284153005464481</c:v>
+                  <c:v>0.994535519125683</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.264339152119701</c:v>
+                  <c:v>0.997506234413965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.047729022324865</c:v>
+                  <c:v>0.996920708237105</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.195933456561922</c:v>
+                  <c:v>1.040665434380776</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.584045584045584</c:v>
+                  <c:v>0.978632478632479</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.210386151797603</c:v>
+                  <c:v>1.007989347536618</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.680154142581888</c:v>
+                  <c:v>1.059730250481696</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.150561797752809</c:v>
+                  <c:v>1.033707865168539</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.095163806552262</c:v>
+                  <c:v>0.992199687987519</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.374558303886926</c:v>
+                  <c:v>1.118374558303887</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.128358208955224</c:v>
+                  <c:v>1.001492537313433</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.268221574344023</c:v>
+                  <c:v>0.994169096209913</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.849869451697128</c:v>
+                  <c:v>0.989120974760661</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.075595727198028</c:v>
+                  <c:v>0.997534921939195</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.303731809399346</c:v>
+                  <c:v>1.020325420015496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,10 +782,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-              </a:schemeClr>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -906,11 +923,168 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="254577544"/>
-        <c:axId val="254435336"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance-SPEC2006'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AddressSanitizer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance-SPEC2006'!$H$2:$H$22</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>400.perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>401.bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>403.gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>429.mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>445.gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>456.hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>458.sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>462.libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>464.h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>471.omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>473.astar</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>483.xalancbmk</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>433.milc</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>444.namd</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>447.dealII</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>450.soplex</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>453.povray</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>470.lbm</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>482.sphinx3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance-SPEC2006'!$L$2:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2.303333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.231372549019608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.761047463175123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.048458149779736</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.21762349799733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.284153005464481</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.264339152119701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.047729022324865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.195933456561922</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.584045584045584</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.210386151797603</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.680154142581888</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.150561797752809</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.095163806552262</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.374558303886926</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.128358208955224</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.268221574344023</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.849869451697128</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.075595727198028</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.303731809399346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="422746392"/>
+        <c:axId val="422729608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254577544"/>
+        <c:axId val="422746392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,19 +1095,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254435336"/>
+        <c:crossAx val="422729608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254435336"/>
+        <c:axId val="422729608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -947,10 +1121,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Normalized Runtime</a:t>
                 </a:r>
               </a:p>
@@ -960,7 +1134,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254577544"/>
+        <c:crossAx val="422746392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -968,6 +1142,16 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1314,11 +1498,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="254650744"/>
-        <c:axId val="254668328"/>
+        <c:axId val="422664712"/>
+        <c:axId val="422649032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254650744"/>
+        <c:axId val="422664712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,14 +1518,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254668328"/>
+        <c:crossAx val="422649032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254668328"/>
+        <c:axId val="422649032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -1368,7 +1552,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254650744"/>
+        <c:crossAx val="422664712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1433,8 +1617,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -1567,6 +1752,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1582,17 +1770,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AddressSanitizer</c:v>
+                  <c:v>DOUBLETAKE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -1670,64 +1855,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.257495144506203</c:v>
+                  <c:v>3.013863692492507</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.173448936060117</c:v>
+                  <c:v>1.153766191951888</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.354611859317659</c:v>
+                  <c:v>2.315939725963255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.136533414121876</c:v>
+                  <c:v>1.162044144335723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.858191054042614</c:v>
+                  <c:v>2.031007478481727</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.70240828081306</c:v>
+                  <c:v>5.390625652155766</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.228009698974233</c:v>
+                  <c:v>1.13737792477708</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.191622591038969</c:v>
+                  <c:v>1.989026688552496</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.751762894534257</c:v>
+                  <c:v>3.804387990762124</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.123188363737673</c:v>
+                  <c:v>1.690549019380227</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.772459837638642</c:v>
+                  <c:v>1.432690315081947</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.681515516581216</c:v>
+                  <c:v>1.869561258510072</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.450165021247834</c:v>
+                  <c:v>1.319383345437288</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.704451267956454</c:v>
+                  <c:v>1.978785080844302</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.855087402659032</c:v>
+                  <c:v>3.3597337077865</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.512751349256181</c:v>
+                  <c:v>3.751235920928261</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34.24271099744246</c:v>
+                  <c:v>12.79462915601023</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.185537008565781</c:v>
+                  <c:v>1.124070130539826</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.001940634234552</c:v>
+                  <c:v>2.170378864728973</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.746520593301515</c:v>
+                  <c:v>2.81521348888001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,17 +1927,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DOUBLETAKE</c:v>
+                  <c:v>AddressSanitizer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
@@ -1830,74 +2012,74 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.013863692492507</c:v>
+                  <c:v>2.257495144506203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.153766191951888</c:v>
+                  <c:v>1.173448936060117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.315939725963255</c:v>
+                  <c:v>3.354611859317659</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.162044144335723</c:v>
+                  <c:v>1.136533414121876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.031007478481727</c:v>
+                  <c:v>4.858191054042614</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.390625652155766</c:v>
+                  <c:v>10.70240828081306</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.13737792477708</c:v>
+                  <c:v>1.228009698974233</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.989026688552496</c:v>
+                  <c:v>2.191622591038969</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.804387990762124</c:v>
+                  <c:v>2.751762894534257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.690549019380227</c:v>
+                  <c:v>3.123188363737673</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.432690315081947</c:v>
+                  <c:v>2.772459837638642</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.869561258510072</c:v>
+                  <c:v>2.681515516581216</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.319383345437288</c:v>
+                  <c:v>1.450165021247834</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.978785080844302</c:v>
+                  <c:v>1.704451267956454</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.3597337077865</c:v>
+                  <c:v>4.855087402659032</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.751235920928261</c:v>
+                  <c:v>4.512751349256181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.79462915601023</c:v>
+                  <c:v>34.24271099744246</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.124070130539826</c:v>
+                  <c:v>1.185537008565781</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.170378864728973</c:v>
+                  <c:v>4.001940634234552</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.81521348888001</c:v>
+                  <c:v>4.746520593301515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="254718280"/>
-        <c:axId val="254723608"/>
+        <c:axId val="422593640"/>
+        <c:axId val="422584600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254718280"/>
+        <c:axId val="422593640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1908,19 +2090,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1"/>
+              <a:defRPr sz="1200" b="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254723608"/>
+        <c:crossAx val="422584600"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254723608"/>
+        <c:axId val="422584600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1935,19 +2117,29 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600"/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
-                  <a:t>Normalized Runtime</a:t>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Normalized </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Memory Usage</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254718280"/>
+        <c:crossAx val="422593640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -1956,6 +2148,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.806700673285404"/>
+          <c:y val="0.151058982210557"/>
+          <c:w val="0.173009471642132"/>
+          <c:h val="0.318252405949256"/>
+        </c:manualLayout>
+      </c:layout>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2410,11 +2612,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="254770520"/>
-        <c:axId val="254761560"/>
+        <c:axId val="456589912"/>
+        <c:axId val="456580952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="254770520"/>
+        <c:axId val="456589912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,14 +2632,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254761560"/>
+        <c:crossAx val="456580952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254761560"/>
+        <c:axId val="456580952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2462,7 +2664,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254770520"/>
+        <c:crossAx val="456589912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2490,7 +2692,7 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2940,10 +3142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView showRuler="0" view="pageLayout" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2952,49 +3154,51 @@
     <col min="6" max="6" width="10.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="B1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
+        <v>80</v>
+      </c>
+      <c r="I1" t="str">
+        <f>D1</f>
+        <v>OD</v>
       </c>
       <c r="J1" t="str">
-        <f>C1</f>
-        <v>AddressSanitizer</v>
+        <f>E1</f>
+        <v>OD+LD</v>
       </c>
       <c r="K1" t="str">
         <f>G1</f>
         <v>DOUBLETAKE</v>
       </c>
-      <c r="L1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" t="s">
-        <v>53</v>
+      <c r="L1" t="str">
+        <f>C1</f>
+        <v>AddressSanitizer</v>
       </c>
       <c r="N1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>600</v>
@@ -3005,6 +3209,9 @@
       <c r="D2">
         <v>811</v>
       </c>
+      <c r="E2">
+        <v>784</v>
+      </c>
       <c r="F2" s="6">
         <v>12313.77</v>
       </c>
@@ -3012,34 +3219,35 @@
         <v>1058</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <f>D2/B2</f>
+        <v>1.3516666666666666</v>
       </c>
       <c r="J2">
-        <f>C2/B2</f>
-        <v>2.3033333333333332</v>
+        <f>E2/B2</f>
+        <v>1.3066666666666666</v>
       </c>
       <c r="K2">
         <f>G2/B2</f>
         <v>1.7633333333333334</v>
       </c>
       <c r="L2">
-        <f>D2/B2</f>
-        <v>1.3516666666666666</v>
-      </c>
-      <c r="M2">
+        <f>C2/B2</f>
+        <v>2.3033333333333332</v>
+      </c>
+      <c r="N2">
         <f>F2/B2</f>
         <v>20.522950000000002</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.35</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>765</v>
@@ -3060,35 +3268,36 @@
         <v>736</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <f t="shared" ref="I3:I20" si="0">D3/B3</f>
+        <v>0.96209150326797388</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J20" si="0">C3/B3</f>
+        <f t="shared" ref="J3:J20" si="1">E3/B3</f>
+        <v>0.96339869281045754</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K20" si="2">G3/B3</f>
+        <v>0.96209150326797388</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L20" si="3">C3/B3</f>
         <v>1.2313725490196079</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K20" si="1">G3/B3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N20" si="4">F3/B3</f>
+        <v>16.820091503267975</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O20" si="5">G3/B3</f>
         <v>0.96209150326797388</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L20" si="2">D3/B3</f>
-        <v>0.96209150326797388</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M20" si="3">F3/B3</f>
-        <v>16.820091503267975</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N20" si="4">G3/B3</f>
-        <v>0.96209150326797388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>611</v>
@@ -3109,34 +3318,35 @@
         <v>868</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.97054009819967269</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0.97054009819967269</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>1.4206219312602291</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>1.7610474631751227</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>18.694909983633387</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.7610474631751227</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>1.4206219312602291</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.97054009819967269</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>18.694909983633387</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>681</v>
@@ -3160,32 +3370,33 @@
         <v>70</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.94713656387665202</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.94566813509544789</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0.94126284875183552</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
         <v>1.0484581497797356</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.94126284875183552</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>0.94713656387665202</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>4.5096769456681356</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
+        <v>4.5096769456681356</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
         <v>0.94126284875183552</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>749</v>
@@ -3209,32 +3420,33 @@
         <v>71</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99732977303070758</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.2176234979973297</v>
-      </c>
-      <c r="K6">
         <f t="shared" si="1"/>
         <v>0.99732977303070758</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <f t="shared" si="2"/>
         <v>0.99732977303070758</v>
       </c>
-      <c r="M6">
+      <c r="L6">
         <f t="shared" si="3"/>
-        <v>28.898344459279038</v>
+        <v>1.2176234979973297</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
+        <v>28.898344459279038</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
         <v>0.99732977303070758</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>915</v>
@@ -3255,35 +3467,36 @@
         <v>911</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99453551912568305</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.99453551912568305</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.99562841530054647</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
         <v>1.284153005464481</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0.99562841530054647</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>0.99453551912568305</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>13.724830601092895</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
+        <v>13.724830601092895</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
         <v>0.99562841530054647</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>802</v>
@@ -3304,35 +3517,36 @@
         <v>800</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99750623441396513</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1.2643391521197007</v>
-      </c>
-      <c r="K8">
         <f t="shared" si="1"/>
         <v>0.99750623441396513</v>
       </c>
-      <c r="L8">
+      <c r="K8">
         <f t="shared" si="2"/>
         <v>0.99750623441396513</v>
       </c>
-      <c r="M8">
+      <c r="L8">
         <f t="shared" si="3"/>
-        <v>20.317955112219451</v>
+        <v>1.2643391521197007</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
+        <v>20.317955112219451</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
         <v>0.99750623441396513</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>1299</v>
@@ -3350,35 +3564,36 @@
         <v>1295</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99692070823710544</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>1.0477290223248652</v>
-      </c>
-      <c r="K9">
         <f t="shared" si="1"/>
         <v>0.99692070823710544</v>
       </c>
-      <c r="L9">
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>0.99692070823710544</v>
       </c>
-      <c r="M9">
+      <c r="L9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.0477290223248652</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
         <v>0.99692070823710544</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>1082</v>
@@ -3396,38 +3611,39 @@
         <v>1378</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.0369685767097967</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1.0406654343807764</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1.2735674676524953</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
         <v>1.1959334565619224</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>1.2735674676524953</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>1.0369685767097967</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
+      <c r="N10">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N10">
-        <f>O10/B10</f>
+      <c r="O10">
+        <f>P10/B10</f>
         <v>1.0406654343807764</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>1126</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>702</v>
@@ -3448,38 +3664,39 @@
         <v>757</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.97008547008547008</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.9786324786324786</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>1.0783475783475784</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
         <v>1.584045584045584</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>1.0783475783475784</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.97008547008547008</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
+      <c r="N11">
+        <f t="shared" si="4"/>
         <v>13.931623931623932</v>
       </c>
-      <c r="N11">
-        <f>O11/B11</f>
+      <c r="O11">
+        <f>P11/B11</f>
         <v>0.97150997150997154</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>682</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>751</v>
@@ -3500,35 +3717,36 @@
         <v>758</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.007989347536618</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1.007989347536618</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>1.0093209054593875</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
         <v>1.2103861517976031</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>1.0093209054593875</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>1.007989347536618</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>11.977363515312916</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
+        <v>11.977363515312916</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
         <v>1.0093209054593875</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>519</v>
@@ -3549,38 +3767,39 @@
         <v>605</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.0520231213872833</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1.0597302504816957</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>1.1657032755298651</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
         <v>1.6801541425818882</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>1.1657032755298651</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>24.04238921001927</v>
+      </c>
+      <c r="O13">
+        <f>P13/B13</f>
         <v>1.0520231213872833</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>24.04238921001927</v>
-      </c>
-      <c r="N13">
-        <f>O13/B13</f>
-        <v>1.0520231213872833</v>
-      </c>
-      <c r="O13">
+      <c r="P13">
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>890</v>
@@ -3601,35 +3820,36 @@
         <v>921</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.0337078651685394</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1.0337078651685394</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1.0348314606741573</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
         <v>1.1505617977528091</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>1.0348314606741573</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>1.0337078651685394</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>11.017988764044944</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
+        <v>11.017988764044944</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
         <v>1.0348314606741573</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>641</v>
@@ -3650,35 +3870,36 @@
         <v>637</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99219968798751945</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.99219968798751945</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0.99375975039001563</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
         <v>1.0951638065522622</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>0.99375975039001563</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>0.99219968798751945</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="3"/>
-        <v>24.893915756630264</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
+        <v>24.893915756630264</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="5"/>
         <v>0.99375975039001563</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>566</v>
@@ -3699,38 +3920,39 @@
         <v>643</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.11660777385159</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1.1183745583038869</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>1.1360424028268552</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
         <v>1.3745583038869258</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>1.1360424028268552</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>1.11660777385159</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
+      <c r="N16">
+        <f t="shared" si="4"/>
         <v>42.828621908127211</v>
       </c>
-      <c r="N16">
-        <f>O16/B16</f>
+      <c r="O16">
+        <f>P16/B16</f>
         <v>1.1183745583038869</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>633</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>670</v>
@@ -3748,35 +3970,36 @@
         <v>670</v>
       </c>
       <c r="H17" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1.0014925373134329</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>1.0014925373134329</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
+      <c r="L17">
+        <f t="shared" si="3"/>
         <v>1.128358208955224</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>1.0014925373134329</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>343</v>
@@ -3794,35 +4017,36 @@
         <v>344</v>
       </c>
       <c r="H18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.99416909620991256</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.99416909620991256</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>1.0029154518950438</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
         <v>1.2682215743440233</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>1.0029154518950438</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0.99416909620991256</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="5"/>
         <v>1.0029154518950438</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>2298</v>
@@ -3840,35 +4064,36 @@
         <v>2273</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.98955613577023493</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
-        <v>0.84986945169712791</v>
-      </c>
-      <c r="K19">
         <f t="shared" si="1"/>
         <v>0.98912097476066141</v>
       </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>0.98912097476066141</v>
+      </c>
       <c r="L19">
-        <f t="shared" si="2"/>
-        <v>0.98955613577023493</v>
-      </c>
-      <c r="M19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.84986945169712791</v>
       </c>
       <c r="N19">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="5"/>
         <v>0.98912097476066141</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>1217</v>
@@ -3886,33 +4111,34 @@
         <v>1228</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.9975349219391948</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0.9975349219391948</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>1.0090386195562859</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
         <v>1.0755957271980279</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>1.0090386195562859</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="2"/>
-        <v>0.9975349219391948</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="N20">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="5"/>
         <v>1.0090386195562859</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="C22">
         <f>SUM(C2:C20)</f>
         <v>19720</v>
@@ -3922,15 +4148,15 @@
         <v>17270</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I22">
         <f>AVERAGE(I2:I20)</f>
-        <v>1</v>
+        <v>1.0215821895146326</v>
       </c>
       <c r="J22">
         <f>AVERAGE(J2:J20)</f>
-        <v>1.3037318093993457</v>
+        <v>1.0203254200154959</v>
       </c>
       <c r="K22">
         <f>AVERAGE(K2:K20)</f>
@@ -3938,36 +4164,37 @@
       </c>
       <c r="L22">
         <f>AVERAGE(L2:L20)</f>
-        <v>1.0215821895146326</v>
-      </c>
-      <c r="N22">
-        <f>AVERAGE(N2:N20)</f>
+        <v>1.3037318093993457</v>
+      </c>
+      <c r="O22">
+        <f>AVERAGE(O2:O20)</f>
         <v>1.0243315648062952</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="G23" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="J23">
+        <f>GEOMEAN(J2:J20)</f>
+        <v>1.0177535796717572</v>
       </c>
       <c r="K23">
         <f>GEOMEAN(K2:K20)</f>
         <v>1.078896726463868</v>
       </c>
-      <c r="L23">
-        <f>GEOMEAN(L2:L20)</f>
-        <v>1.018465273620357</v>
-      </c>
-      <c r="N23">
-        <f>GEOMEAN(N2:N20)</f>
+      <c r="O23">
+        <f>GEOMEAN(O2:O20)</f>
         <v>1.0212793102633213</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="G24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3984,7 +4211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView showRuler="0" view="pageLayout" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3997,22 +4224,22 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I1" t="str">
         <f>C1</f>
@@ -4027,12 +4254,12 @@
         <v>Use-After-FreeDetection</v>
       </c>
       <c r="L1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>600</v>
@@ -4050,7 +4277,7 @@
         <v>1058</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -4074,7 +4301,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>611</v>
@@ -4092,7 +4319,7 @@
         <v>868</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -4116,7 +4343,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>1082</v>
@@ -4134,7 +4361,7 @@
         <v>1378</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -4158,7 +4385,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>702</v>
@@ -4176,7 +4403,7 @@
         <v>757</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -4200,7 +4427,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>519</v>
@@ -4218,7 +4445,7 @@
         <v>605</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -4242,7 +4469,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>566</v>
@@ -4260,7 +4487,7 @@
         <v>643</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -4288,7 +4515,7 @@
         <v>4391</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H9">
         <f>AVERAGE(H2:H7)</f>
@@ -4313,7 +4540,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B38">
         <v>655958</v>
@@ -4324,7 +4551,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <v>683412</v>
@@ -4335,7 +4562,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>64950</v>
@@ -4346,7 +4573,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>172289</v>
@@ -4357,7 +4584,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>428316</v>
@@ -4368,7 +4595,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>514172</v>
@@ -4378,6 +4605,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4392,10 +4620,150 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView showRuler="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22">
+        <f>SUM(B2:B20)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showRuler="0" view="pageLayout" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4406,33 +4774,35 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="G1" t="str">
+        <f>D1</f>
+        <v>DOUBLETAKE</v>
+      </c>
+      <c r="H1" s="8" t="str">
+        <f>C1</f>
+        <v>AddressSanitizer</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>655958</v>
@@ -4451,12 +4821,12 @@
         <v>1</v>
       </c>
       <c r="G2">
+        <f>D2/B2</f>
+        <v>3.0138636924925071</v>
+      </c>
+      <c r="H2" s="8">
         <f>C2/B2</f>
         <v>2.257495144506203</v>
-      </c>
-      <c r="H2" s="8">
-        <f t="shared" ref="H2:H20" si="0">D2/B2</f>
-        <v>3.0138636924925071</v>
       </c>
       <c r="I2">
         <f>C2/B2</f>
@@ -4466,13 +4836,13 @@
         <v>2027588</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K20" si="1">J2/B2</f>
+        <f t="shared" ref="K2:K20" si="0">J2/B2</f>
         <v>3.0910332673738257</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>869645</v>
@@ -4484,19 +4854,19 @@
         <v>1003367</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E20" si="2">A3</f>
+        <f t="shared" ref="E3:E20" si="1">A3</f>
         <v>401.bzip2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G20" si="3">C3/B3</f>
+        <f t="shared" ref="G3:G20" si="2">D3/B3</f>
+        <v>1.1537661919518885</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:H20" si="3">C3/B3</f>
         <v>1.1734489360601166</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1537661919518885</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I20" si="4">C3/B3</f>
@@ -4506,13 +4876,13 @@
         <v>1140444</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3113902799418153</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>683412</v>
@@ -4524,19 +4894,19 @@
         <v>1582741</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>403.gcc</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
+        <f t="shared" si="2"/>
+        <v>2.315939725963255</v>
+      </c>
+      <c r="H4" s="8">
         <f t="shared" si="3"/>
         <v>3.354611859317659</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="0"/>
-        <v>2.315939725963255</v>
       </c>
       <c r="I4">
         <f t="shared" si="4"/>
@@ -4546,13 +4916,13 @@
         <v>1452497</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.1253606901839595</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>1716415</v>
@@ -4564,19 +4934,19 @@
         <v>1994550</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>429.mcf</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1.162044144335723</v>
+      </c>
+      <c r="H5" s="8">
         <f t="shared" si="3"/>
         <v>1.1365334141218761</v>
-      </c>
-      <c r="H5" s="8">
-        <f t="shared" si="0"/>
-        <v>1.162044144335723</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
@@ -4586,13 +4956,13 @@
         <v>2177862</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.268843490647658</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>28348</v>
@@ -4604,19 +4974,19 @@
         <v>57575</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>445.gobmk</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
+        <f t="shared" si="2"/>
+        <v>2.0310074784817269</v>
+      </c>
+      <c r="H6" s="8">
         <f t="shared" si="3"/>
         <v>4.8581910540426136</v>
-      </c>
-      <c r="H6" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0310074784817269</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
@@ -4626,13 +4996,13 @@
         <v>97015</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.4222872865810641</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>23959</v>
@@ -4644,19 +5014,19 @@
         <v>129154</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>456.hmmer</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
+        <f t="shared" si="2"/>
+        <v>5.3906256521557658</v>
+      </c>
+      <c r="H7" s="8">
         <f t="shared" si="3"/>
         <v>10.702408280813057</v>
-      </c>
-      <c r="H7" s="8">
-        <f t="shared" si="0"/>
-        <v>5.3906256521557658</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
@@ -4666,13 +5036,13 @@
         <v>226833</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.4675487290788425</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>178988</v>
@@ -4684,19 +5054,19 @@
         <v>203577</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>458.sjeng</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1.1373779247770801</v>
+      </c>
+      <c r="H8" s="8">
         <f t="shared" si="3"/>
         <v>1.2280096989742328</v>
-      </c>
-      <c r="H8" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1373779247770801</v>
       </c>
       <c r="I8">
         <f t="shared" si="4"/>
@@ -4706,13 +5076,13 @@
         <v>260522</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4555277448767514</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>65796</v>
@@ -4724,32 +5094,32 @@
         <v>130870</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>462.libquantum</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1.9890266885524956</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="3"/>
         <v>2.1916225910389691</v>
-      </c>
-      <c r="H9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.9890266885524956</v>
       </c>
       <c r="I9">
         <f t="shared" si="4"/>
         <v>2.1916225910389691</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>64950</v>
@@ -4761,32 +5131,32 @@
         <v>247095</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>464.h264ref</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
+        <f t="shared" si="2"/>
+        <v>3.8043879907621245</v>
+      </c>
+      <c r="H10" s="8">
         <f t="shared" si="3"/>
         <v>2.7517628945342572</v>
-      </c>
-      <c r="H10" s="8">
-        <f t="shared" si="0"/>
-        <v>3.8043879907621245</v>
       </c>
       <c r="I10">
         <f t="shared" si="4"/>
         <v>2.7517628945342572</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>172289</v>
@@ -4798,19 +5168,19 @@
         <v>291263</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>471.omnetpp</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
+        <f t="shared" si="2"/>
+        <v>1.6905490193802275</v>
+      </c>
+      <c r="H11" s="8">
         <f t="shared" si="3"/>
         <v>3.1231883637376732</v>
-      </c>
-      <c r="H11" s="8">
-        <f t="shared" si="0"/>
-        <v>1.6905490193802275</v>
       </c>
       <c r="I11">
         <f t="shared" si="4"/>
@@ -4820,13 +5190,13 @@
         <v>626328</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.6353336544991266</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>332961</v>
@@ -4838,19 +5208,19 @@
         <v>477030</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>473.astar</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
+        <f t="shared" si="2"/>
+        <v>1.4326903150819466</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="3"/>
         <v>2.7724598376386425</v>
-      </c>
-      <c r="H12" s="8">
-        <f t="shared" si="0"/>
-        <v>1.4326903150819466</v>
       </c>
       <c r="I12">
         <f t="shared" si="4"/>
@@ -4860,13 +5230,13 @@
         <v>547175</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6433606338279858</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>428316</v>
@@ -4878,19 +5248,19 @@
         <v>800763</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>483.xalancbmk</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1.869561258510072</v>
+      </c>
+      <c r="H13" s="8">
         <f t="shared" si="3"/>
         <v>2.6815155165812157</v>
-      </c>
-      <c r="H13" s="8">
-        <f t="shared" si="0"/>
-        <v>1.869561258510072</v>
       </c>
       <c r="I13">
         <f t="shared" si="4"/>
@@ -4900,13 +5270,13 @@
         <v>874879</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.0426017239608139</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>695365</v>
@@ -4918,19 +5288,19 @@
         <v>917453</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>433.milc</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1.3193833454372883</v>
+      </c>
+      <c r="H14" s="8">
         <f t="shared" si="3"/>
         <v>1.4501650212478339</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" si="0"/>
-        <v>1.3193833454372883</v>
       </c>
       <c r="I14">
         <f t="shared" si="4"/>
@@ -4940,13 +5310,13 @@
         <v>934978</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3445859368820692</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>46571</v>
@@ -4958,19 +5328,19 @@
         <v>92154</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>444.namd</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1.9787850808443022</v>
+      </c>
+      <c r="H15" s="8">
         <f t="shared" si="3"/>
         <v>1.7044512679564536</v>
-      </c>
-      <c r="H15" s="8">
-        <f t="shared" si="0"/>
-        <v>1.9787850808443022</v>
       </c>
       <c r="I15">
         <f t="shared" si="4"/>
@@ -4980,13 +5350,13 @@
         <v>131123</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.8155504498507655</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>514172</v>
@@ -4998,32 +5368,32 @@
         <v>1727481</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>447.dealII</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
+        <f t="shared" si="2"/>
+        <v>3.3597337077864995</v>
+      </c>
+      <c r="H16" s="8">
         <f t="shared" si="3"/>
         <v>4.8550874026590325</v>
-      </c>
-      <c r="H16" s="8">
-        <f t="shared" si="0"/>
-        <v>3.3597337077864995</v>
       </c>
       <c r="I16">
         <f t="shared" si="4"/>
         <v>4.8550874026590325</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>441169</v>
@@ -5035,32 +5405,32 @@
         <v>1654929</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>450.soplex</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
+        <f t="shared" si="2"/>
+        <v>3.7512359209282611</v>
+      </c>
+      <c r="H17" s="8">
         <f t="shared" si="3"/>
         <v>4.512751349256181</v>
-      </c>
-      <c r="H17" s="8">
-        <f t="shared" si="0"/>
-        <v>3.7512359209282611</v>
       </c>
       <c r="I17">
         <f t="shared" si="4"/>
         <v>4.512751349256181</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>3910</v>
@@ -5072,32 +5442,32 @@
         <v>50027</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>453.povray</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
+        <f t="shared" si="2"/>
+        <v>12.794629156010231</v>
+      </c>
+      <c r="H18" s="8">
         <f t="shared" si="3"/>
         <v>34.242710997442458</v>
-      </c>
-      <c r="H18" s="8">
-        <f t="shared" si="0"/>
-        <v>12.794629156010231</v>
       </c>
       <c r="I18">
         <f t="shared" si="4"/>
         <v>34.242710997442458</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>418876</v>
@@ -5109,32 +5479,32 @@
         <v>470846</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>470.lbm</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
+        <f t="shared" si="2"/>
+        <v>1.1240701305398255</v>
+      </c>
+      <c r="H19" s="8">
         <f t="shared" si="3"/>
         <v>1.1855370085657808</v>
-      </c>
-      <c r="H19" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1240701305398255</v>
       </c>
       <c r="I19">
         <f t="shared" si="4"/>
         <v>1.1855370085657808</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>45346</v>
@@ -5146,26 +5516,26 @@
         <v>98418</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>482.sphinx3</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
+        <f t="shared" si="2"/>
+        <v>2.1703788647289728</v>
+      </c>
+      <c r="H20" s="8">
         <f t="shared" si="3"/>
         <v>4.0019406342345523</v>
-      </c>
-      <c r="H20" s="8">
-        <f t="shared" si="0"/>
-        <v>2.1703788647289728</v>
       </c>
       <c r="I20">
         <f t="shared" si="4"/>
         <v>4.0019406342345523</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -5183,15 +5553,18 @@
         <v>13906261</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
       </c>
       <c r="G22">
         <f>AVERAGE(G2:G20)</f>
-        <v>4.7465205933015158</v>
+        <v>2.8152134888800098</v>
       </c>
       <c r="H22" s="8">
         <f>AVERAGE(H2:H20)</f>
-        <v>2.8152134888800098</v>
+        <v>4.7465205933015158</v>
       </c>
       <c r="I22">
         <f>AVERAGE(I2:I20)</f>
@@ -5211,7 +5584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -5227,35 +5600,35 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="E2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0.5</v>
@@ -5267,7 +5640,7 @@
         <v>0.62</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -5283,7 +5656,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -5295,7 +5668,7 @@
         <v>11.11</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -5311,7 +5684,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.23</v>
@@ -5323,7 +5696,7 @@
         <v>0.34</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -5339,7 +5712,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>18.87</v>
@@ -5351,7 +5724,7 @@
         <v>18.579999999999998</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -5367,7 +5740,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>19.989999999999998</v>
@@ -5379,7 +5752,7 @@
         <v>21.55</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -5395,7 +5768,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>2.14</v>
@@ -5407,7 +5780,7 @@
         <v>3.01</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -5423,7 +5796,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0.25900000000000001</v>
@@ -5435,7 +5808,7 @@
         <v>0.27</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -5451,7 +5824,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>2.629</v>
@@ -5463,7 +5836,7 @@
         <v>3.05</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -5479,15 +5852,15 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>10.16</v>
@@ -5499,7 +5872,7 @@
         <v>10.25</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -5515,7 +5888,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>1.92</v>
@@ -5527,7 +5900,7 @@
         <v>2.8</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -5543,7 +5916,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>5.9</v>
@@ -5555,7 +5928,7 @@
         <v>5.69</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -5571,7 +5944,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>1.84</v>
@@ -5583,7 +5956,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -5599,7 +5972,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>2.78</v>
@@ -5611,7 +5984,7 @@
         <v>4.22</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -5627,7 +6000,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>4.4189999999999996</v>
@@ -5639,7 +6012,7 @@
         <v>6.35</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -5655,7 +6028,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>0.98</v>
@@ -5667,7 +6040,7 @@
         <v>1.06</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -5683,7 +6056,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="E20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -5708,24 +6081,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showRuler="0" view="pageLayout" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>